<commit_message>
新增Websocket 支援/ TCP API 支援
</commit_message>
<xml_diff>
--- a/現場出差測試/20230323-UMTC.xlsx
+++ b/現場出差測試/20230323-UMTC.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\專案\AGV\GPMCasstteConvertCIM\現場出差測試\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84098DD-C492-472B-82DC-A4005D2870B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>交握IO點位測試</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISSUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +63,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -45,15 +111,171 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +552,318 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="7" customWidth="1"/>
+    <col min="4" max="5" width="45.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>21</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>23</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>25</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>26</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8">
+        <v>27</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>